<commit_message>
Update 0706: Change ID of objects 01_Destination_Table> 01-btn_Add 01_Destination_Table> 05-btn_AddDestination
</commit_message>
<xml_diff>
--- a/Test Data/Happy Path/NCABT.xlsx
+++ b/Test Data/Happy Path/NCABT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elijah Siason\Katalon Studio\NCABT\Test Data\Happy Path\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asllie Sablan\Katalon Studio\GIT\NCABT_Repo\Test Data\Happy Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C92BBB0A-3BDA-4D3A-9B09-5C9957680884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247EC2DC-A66F-4C33-9197-3418C3E4C976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C64871BC-84E5-4822-B28F-C4706A458858}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C64871BC-84E5-4822-B28F-C4706A458858}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>NA_BusinessName</t>
   </si>
@@ -123,9 +123,6 @@
     <t>$750 DED</t>
   </si>
   <si>
-    <t>$300/600</t>
-  </si>
-  <si>
     <t>$5K W/500 DED</t>
   </si>
   <si>
@@ -168,15 +165,15 @@
     <t>California</t>
   </si>
   <si>
+    <t>20,001 - 45,000</t>
+  </si>
+  <si>
     <t>Full size Van</t>
   </si>
   <si>
     <t>$500 DED</t>
   </si>
   <si>
-    <t>$1,500 DED</t>
-  </si>
-  <si>
     <t>V_BusinessClass</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>HC_TotalFleetMileage</t>
   </si>
   <si>
-    <t>03102020</t>
-  </si>
-  <si>
     <t>CH_LossRunDate</t>
   </si>
   <si>
@@ -279,31 +273,22 @@
     <t>RS_GLPayroll</t>
   </si>
   <si>
-    <t>0 - 10,000</t>
-  </si>
-  <si>
-    <t>HC_CollisionDeductible</t>
-  </si>
-  <si>
-    <t>HC_CompreDeductible</t>
-  </si>
-  <si>
-    <t>StateNJ</t>
+    <t>05012020</t>
+  </si>
+  <si>
+    <t>Commercial</t>
   </si>
   <si>
     <t>Courier</t>
   </si>
   <si>
-    <t>L_PIP</t>
-  </si>
-  <si>
-    <t>$250,000 PRIMARY W/$2,000 DED</t>
-  </si>
-  <si>
-    <t>L_PIPSymbol</t>
-  </si>
-  <si>
-    <t>2) All Owned Autos</t>
+    <t>$300,000/600,000</t>
+  </si>
+  <si>
+    <t>$1,000 DED</t>
+  </si>
+  <si>
+    <t>Smoke Test</t>
   </si>
 </sst>
 </file>
@@ -311,7 +296,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -360,14 +345,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,73 +666,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80686887-9963-428D-9676-5B1BD08873B8}">
-  <dimension ref="A1:BG2"/>
+  <dimension ref="A1:BC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BG2" sqref="BG2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.7109375" customWidth="1"/>
-    <col min="50" max="50" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,313 +775,289 @@
       <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>88</v>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
       </c>
       <c r="X1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Z1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AA1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="AB1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="AC1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AE1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AF1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="AH1" t="s">
         <v>37</v>
       </c>
       <c r="AI1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL1" t="s">
         <v>47</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2010</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2">
+        <v>20001</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="U2" s="3">
+        <v>50000</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AN1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BE1" t="s">
+      <c r="AM2" s="2">
+        <v>10111990</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>12500</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>11012020</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BF1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>2010</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>1500000</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="U2" s="5">
-        <v>2000</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" s="4">
-        <v>2000</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL2" s="4">
-        <v>20000</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO2" s="4">
-        <v>10111990</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ2" s="4">
-        <v>7</v>
-      </c>
-      <c r="AR2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AS2" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="AT2" s="4">
+      <c r="AW2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AX2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AY2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AZ2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>10</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>10</v>
+      </c>
+      <c r="BC2" s="2">
         <v>15000</v>
-      </c>
-      <c r="AU2" s="4">
-        <v>200</v>
-      </c>
-      <c r="AV2" s="4">
-        <v>1500</v>
-      </c>
-      <c r="AW2" s="4">
-        <v>1500</v>
-      </c>
-      <c r="AX2" s="4">
-        <v>250000</v>
-      </c>
-      <c r="AY2" s="4">
-        <v>12302020</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA2" s="4">
-        <v>10000</v>
-      </c>
-      <c r="BB2" s="4">
-        <v>10000</v>
-      </c>
-      <c r="BC2" s="4">
-        <v>10000</v>
-      </c>
-      <c r="BD2" s="4">
-        <v>400</v>
-      </c>
-      <c r="BE2" s="4">
-        <v>400</v>
-      </c>
-      <c r="BF2" s="4">
-        <v>400</v>
-      </c>
-      <c r="BG2" s="4">
-        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Data update Historical Coverage Object Update
</commit_message>
<xml_diff>
--- a/Test Data/Happy Path/NCABT.xlsx
+++ b/Test Data/Happy Path/NCABT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asllie Sablan\Katalon Studio\GIT\NCABT_Repo\Test Data\Happy Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247EC2DC-A66F-4C33-9197-3418C3E4C976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C7D8A99-AB2D-4784-B4CD-D00A657CAD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C64871BC-84E5-4822-B28F-C4706A458858}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>NA_BusinessName</t>
   </si>
@@ -288,7 +288,13 @@
     <t>$1,000 DED</t>
   </si>
   <si>
-    <t>Smoke Test</t>
+    <t>Smoke Test RIV</t>
+  </si>
+  <si>
+    <t>HC_CollisionDeductible</t>
+  </si>
+  <si>
+    <t>HC_CompreDeductible</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,12 +329,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,13 +345,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80686887-9963-428D-9676-5B1BD08873B8}">
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -714,19 +713,21 @@
     <col min="42" max="42" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.54296875" customWidth="1"/>
+    <col min="46" max="46" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.81640625" customWidth="1"/>
+    <col min="48" max="48" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -863,37 +864,43 @@
         <v>57</v>
       </c>
       <c r="AT1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV1" t="s">
         <v>58</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>59</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>60</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>61</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>62</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>63</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>64</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>65</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>66</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -916,7 +923,7 @@
         <v>76</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>81</v>
@@ -963,7 +970,7 @@
       <c r="W2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="2" t="s">
         <v>82</v>
       </c>
       <c r="Y2" s="2" t="s">
@@ -996,14 +1003,14 @@
       <c r="AH2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AI2" s="2" t="s">
         <v>83</v>
       </c>
       <c r="AJ2" s="2">
         <v>10000</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AL2" s="2" t="s">
         <v>52</v>
@@ -1030,19 +1037,19 @@
         <v>1</v>
       </c>
       <c r="AT2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AV2" s="2">
         <v>12500</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="AW2" s="2">
         <v>11012020</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="AW2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="AX2" s="2">
-        <v>1000</v>
       </c>
       <c r="AY2" s="2">
         <v>1000</v>
@@ -1051,12 +1058,18 @@
         <v>1000</v>
       </c>
       <c r="BA2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BC2" s="2">
         <v>10</v>
       </c>
-      <c r="BB2" s="2">
+      <c r="BD2" s="2">
         <v>10</v>
       </c>
-      <c r="BC2" s="2">
+      <c r="BE2" s="2">
         <v>15000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lower PIP in Limits - update in script Higher Comp FT/Ded - update in Test Data
Added script for:
Bind
Forms Selection
Notes

On Quote Option commented the automation for upload
</commit_message>
<xml_diff>
--- a/Test Data/Happy Path/NCABT.xlsx
+++ b/Test Data/Happy Path/NCABT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asllie Sablan\Katalon Studio\GIT\NCABT_Repo\Test Data\Happy Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C7D8A99-AB2D-4784-B4CD-D00A657CAD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092E3143-575B-43CB-A268-4CCA1069A7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C64871BC-84E5-4822-B28F-C4706A458858}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C64871BC-84E5-4822-B28F-C4706A458858}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>NA_BusinessName</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Full size Van</t>
-  </si>
-  <si>
-    <t>$500 DED</t>
   </si>
   <si>
     <t>V_BusinessClass</t>
@@ -328,7 +325,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,10 +344,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,19 +774,19 @@
         <v>20</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V1" t="s">
         <v>23</v>
@@ -825,7 +822,7 @@
         <v>36</v>
       </c>
       <c r="AG1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AH1" t="s">
         <v>37</v>
@@ -837,239 +834,239 @@
         <v>39</v>
       </c>
       <c r="AK1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2010</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1">
+        <v>20001</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="2">
+        <v>50000</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD1" t="s">
+      <c r="AM2" s="1">
+        <v>10111990</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>15000</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>15000</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>12500</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>11012020</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BE1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2010</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="2">
-        <v>20001</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="U2" s="3">
-        <v>50000</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>10000</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>10111990</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ2" s="2">
-        <v>15000</v>
-      </c>
-      <c r="AR2" s="2">
-        <v>15000</v>
-      </c>
-      <c r="AS2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="2">
+      <c r="AY2" s="1">
         <v>1000</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="AZ2" s="1">
         <v>1000</v>
       </c>
-      <c r="AV2" s="2">
-        <v>12500</v>
-      </c>
-      <c r="AW2" s="2">
-        <v>11012020</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY2" s="2">
+      <c r="BA2" s="1">
         <v>1000</v>
       </c>
-      <c r="AZ2" s="2">
+      <c r="BB2" s="1">
         <v>1000</v>
       </c>
-      <c r="BA2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="BB2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="BC2" s="2">
+      <c r="BC2" s="1">
         <v>10</v>
       </c>
-      <c r="BD2" s="2">
+      <c r="BD2" s="1">
         <v>10</v>
       </c>
-      <c r="BE2" s="2">
+      <c r="BE2" s="1">
         <v>15000</v>
       </c>
     </row>

</xml_diff>